<commit_message>
Updating the excel file with corrected group and naming
</commit_message>
<xml_diff>
--- a/data/_raw/acmap_NA.xlsx
+++ b/data/_raw/acmap_NA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hilarius\OneDrive - Danmarks Tekniske Universitet\Dokumenter\Antigenic-Mapping-of-NA\data\_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliv4107.NEXT\Documents\R\Bachelor\Antigenic-Mapping-of-NA\data\_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A992382-4B56-47E6-A288-5F7D0FDFDAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBA6473-DA3E-4987-8F20-971EE6BA1313}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AntigenicMappingTemplate_ATM_" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="92">
   <si>
     <t>Made by;                                                                OLSE &amp; MAOJ, 2024</t>
   </si>
@@ -222,16 +222,10 @@
     <t>H1N1 A/Denmark/2021/01</t>
   </si>
   <si>
-    <t>Challenge strain for this study</t>
-  </si>
-  <si>
     <t>H6N1 A/CA/04/2009/N1 (H1N1)</t>
   </si>
   <si>
     <t>H6N2 A/Texas/50/2012(4) (H3N2)</t>
-  </si>
-  <si>
-    <t>unrelated NA with Recombinant H6</t>
   </si>
   <si>
     <t>Richard Webby's lab</t>
@@ -268,12 +262,6 @@
   </si>
   <si>
     <t>Group 2</t>
-  </si>
-  <si>
-    <t>HA is recombinant H6, NA is the same as Pandemic 2009 H1N1</t>
-  </si>
-  <si>
-    <t>Group 1???</t>
   </si>
   <si>
     <t>Multiple exposures!?</t>
@@ -323,12 +311,21 @@
   <si>
     <t>Serum exposure antigen:</t>
   </si>
+  <si>
+    <t>Recombinant 2009 H6N1</t>
+  </si>
+  <si>
+    <t>Challenge strain</t>
+  </si>
+  <si>
+    <t>unrelated H6N2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,14 +807,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1166,56 +1163,56 @@
   <dimension ref="A1:KA264"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" style="1" customWidth="1"/>
     <col min="11" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.875" style="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="1" customWidth="1"/>
-    <col min="14" max="22" width="9.1796875" style="1"/>
-    <col min="23" max="23" width="13.453125" style="1" customWidth="1"/>
-    <col min="24" max="60" width="9.1796875" style="1"/>
-    <col min="61" max="61" width="7.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="72" width="9.1796875" style="1"/>
-    <col min="73" max="88" width="10.6328125" style="1" customWidth="1"/>
-    <col min="89" max="16384" width="9.1796875" style="1"/>
+    <col min="14" max="22" width="9.125" style="1"/>
+    <col min="23" max="23" width="13.5" style="1" customWidth="1"/>
+    <col min="24" max="60" width="9.125" style="1"/>
+    <col min="61" max="61" width="7.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="72" width="9.125" style="1"/>
+    <col min="73" max="88" width="10.625" style="1" customWidth="1"/>
+    <col min="89" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:287" s="5" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:287" s="5" customFormat="1" ht="44.25" customHeight="1" thickBot="1">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
     </row>
-    <row r="2" spans="1:287" s="4" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:287" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:287" s="4" customFormat="1" ht="16.5" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:287" ht="16.5" customHeight="1">
       <c r="B3" s="4"/>
       <c r="C3" s="33" t="s">
         <v>2</v>
@@ -1225,13 +1222,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="7"/>
@@ -1513,7 +1510,7 @@
       <c r="JZ3" s="4"/>
       <c r="KA3" s="4"/>
     </row>
-    <row r="4" spans="1:287" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:287" ht="16.5" customHeight="1" thickBot="1">
       <c r="B4" s="4"/>
       <c r="C4" s="35">
         <v>45371</v>
@@ -1801,7 +1798,7 @@
       <c r="JZ4" s="4"/>
       <c r="KA4" s="4"/>
     </row>
-    <row r="5" spans="1:287" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:287" ht="16.5" customHeight="1" thickBot="1">
       <c r="B5" s="4"/>
       <c r="C5" s="7"/>
       <c r="D5" s="4"/>
@@ -1809,13 +1806,13 @@
         <v>5</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="7"/>
@@ -2097,7 +2094,7 @@
       <c r="JZ5" s="4"/>
       <c r="KA5" s="4"/>
     </row>
-    <row r="6" spans="1:287" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:287" ht="16.5" customHeight="1" thickBot="1">
       <c r="B6" s="4"/>
       <c r="C6" s="33" t="s">
         <v>7</v>
@@ -2387,7 +2384,7 @@
       <c r="JZ6" s="4"/>
       <c r="KA6" s="4"/>
     </row>
-    <row r="7" spans="1:287" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:287" ht="18" customHeight="1" thickBot="1">
       <c r="B7" s="4"/>
       <c r="C7" s="34"/>
       <c r="D7" s="4"/>
@@ -2675,7 +2672,7 @@
       <c r="JZ7" s="10"/>
       <c r="KA7" s="10"/>
     </row>
-    <row r="8" spans="1:287" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:287" customFormat="1" ht="24" customHeight="1">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -2692,7 +2689,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
     </row>
-    <row r="9" spans="1:287" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:287" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2700,263 +2697,263 @@
       <c r="E9" s="4"/>
       <c r="F9" s="12"/>
       <c r="G9" s="41" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="T9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="U9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="V9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="W9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="X9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Y9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Z9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AA9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AB9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AC9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AD9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AE9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AF9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AG9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AH9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AI9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AJ9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AK9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AL9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AM9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AN9" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AO9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AP9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AQ9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AR9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AS9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AT9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AU9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AV9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AW9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AX9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AY9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AZ9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BA9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BB9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BC9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BD9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BE9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BF9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BG9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BH9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BI9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BJ9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BK9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BL9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BM9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BN9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BO9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BP9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BQ9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BR9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BS9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BT9" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BU9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="BV9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="BW9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="BX9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="BY9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="BZ9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CA9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CB9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CC9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CD9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CE9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CF9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CG9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CH9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CI9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CJ9" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:287" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:287" ht="27.95" customHeight="1">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="37" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I10" s="32" t="s">
         <v>54</v>
@@ -3055,158 +3052,158 @@
         <v>54</v>
       </c>
       <c r="AO10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AT10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AX10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BC10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BD10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BE10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BN10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BO10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BQ10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BR10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BS10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BT10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BU10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="AP10" s="1" t="s">
+      <c r="BV10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="AQ10" s="1" t="s">
+      <c r="BW10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="AR10" s="1" t="s">
+      <c r="BX10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="AS10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AT10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AU10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AW10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AX10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AY10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AZ10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BA10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BB10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BC10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BD10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BE10" s="1" t="s">
+      <c r="BY10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="BF10" s="1" t="s">
+      <c r="BZ10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="BG10" s="1" t="s">
+      <c r="CA10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="BH10" s="1" t="s">
+      <c r="CB10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="BI10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BJ10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BK10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BL10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BM10" s="1" t="s">
+      <c r="CC10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="BN10" s="1" t="s">
+      <c r="CD10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="BO10" s="1" t="s">
+      <c r="CE10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="BP10" s="1" t="s">
+      <c r="CF10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="BQ10" s="1" t="s">
+      <c r="CG10" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="BR10" s="1" t="s">
+      <c r="CH10" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="BS10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BT10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BU10" s="32" t="s">
+      <c r="CI10" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="BV10" s="32" t="s">
+      <c r="CJ10" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="BW10" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="BX10" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="BY10" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="BZ10" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA10" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="CB10" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="CC10" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="CD10" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="CE10" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="CF10" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="CG10" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="CH10" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="CI10" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="CJ10" s="36" t="s">
-        <v>90</v>
-      </c>
     </row>
-    <row r="11" spans="1:287" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:287" ht="24" customHeight="1" thickBot="1">
       <c r="B11" s="4"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="38" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>10</v>
@@ -3419,7 +3416,7 @@
         <v>26</v>
       </c>
       <c r="BZ11" s="40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="CA11" s="39" t="s">
         <v>31</v>
@@ -3650,7 +3647,7 @@
       <c r="JY11" s="6"/>
       <c r="JZ11" s="6"/>
     </row>
-    <row r="12" spans="1:287" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:287" ht="24.75" customHeight="1" thickTop="1">
       <c r="B12" s="8"/>
       <c r="C12" s="3" t="s">
         <v>11</v>
@@ -3665,7 +3662,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H12" s="42" t="s">
         <v>15</v>
@@ -3949,23 +3946,23 @@
       <c r="JY12" s="4"/>
       <c r="JZ12" s="4"/>
     </row>
-    <row r="13" spans="1:287" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:287">
       <c r="B13" s="8"/>
       <c r="C13" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>57</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G13" s="46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H13" s="43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I13" s="13">
         <v>7.2</v>
@@ -4406,7 +4403,7 @@
       <c r="JY13" s="6"/>
       <c r="JZ13" s="6"/>
     </row>
-    <row r="14" spans="1:287" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:287">
       <c r="B14" s="8"/>
       <c r="C14" s="14" t="s">
         <v>55</v>
@@ -4416,11 +4413,11 @@
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="43" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="I14" s="13">
         <v>16.3</v>
@@ -4861,21 +4858,21 @@
       <c r="JY14" s="6"/>
       <c r="JZ14" s="6"/>
     </row>
-    <row r="15" spans="1:287" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:287" ht="28.5">
       <c r="B15" s="8"/>
       <c r="C15" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G15" s="47"/>
       <c r="H15" s="43" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="I15" s="13">
         <v>33.9</v>
@@ -5316,21 +5313,21 @@
       <c r="JY15" s="6"/>
       <c r="JZ15" s="6"/>
     </row>
-    <row r="16" spans="1:287" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:287" ht="28.5">
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G16" s="47"/>
       <c r="H16" s="43" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="I16" s="13">
         <v>15</v>
@@ -5551,7 +5548,7 @@
       <c r="CC16" s="13">
         <v>15.1</v>
       </c>
-      <c r="CD16" s="51"/>
+      <c r="CD16" s="49"/>
       <c r="CE16" s="13">
         <v>15.1</v>
       </c>
@@ -5769,7 +5766,7 @@
       <c r="JY16" s="6"/>
       <c r="JZ16" s="6"/>
     </row>
-    <row r="17" spans="2:286" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:286" ht="28.5">
       <c r="B17" s="8"/>
       <c r="C17" s="14" t="s">
         <v>55</v>
@@ -5779,10 +5776,10 @@
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H17" s="43" t="s">
         <v>56</v>
@@ -6226,7 +6223,7 @@
       <c r="JY17" s="6"/>
       <c r="JZ17" s="6"/>
     </row>
-    <row r="18" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:286">
       <c r="B18" s="8"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -6513,7 +6510,7 @@
       <c r="JY18" s="6"/>
       <c r="JZ18" s="6"/>
     </row>
-    <row r="19" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:286">
       <c r="B19" s="8"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -6800,7 +6797,7 @@
       <c r="JY19" s="6"/>
       <c r="JZ19" s="6"/>
     </row>
-    <row r="20" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:286">
       <c r="B20" s="8"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -7087,7 +7084,7 @@
       <c r="JY20" s="6"/>
       <c r="JZ20" s="6"/>
     </row>
-    <row r="21" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:286">
       <c r="B21" s="8"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -7374,7 +7371,7 @@
       <c r="JY21" s="6"/>
       <c r="JZ21" s="6"/>
     </row>
-    <row r="22" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:286">
       <c r="B22" s="8"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -7661,7 +7658,7 @@
       <c r="JY22" s="6"/>
       <c r="JZ22" s="6"/>
     </row>
-    <row r="23" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:286">
       <c r="B23" s="8"/>
       <c r="G23" s="47"/>
       <c r="H23" s="44"/>
@@ -7944,7 +7941,7 @@
       <c r="JY23" s="6"/>
       <c r="JZ23" s="6"/>
     </row>
-    <row r="24" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:286">
       <c r="B24" s="8"/>
       <c r="G24" s="47"/>
       <c r="H24" s="44"/>
@@ -8227,7 +8224,7 @@
       <c r="JY24" s="6"/>
       <c r="JZ24" s="6"/>
     </row>
-    <row r="25" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:286">
       <c r="B25" s="8"/>
       <c r="G25" s="47"/>
       <c r="H25" s="44"/>
@@ -8510,7 +8507,7 @@
       <c r="JY25" s="6"/>
       <c r="JZ25" s="6"/>
     </row>
-    <row r="26" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:286">
       <c r="B26" s="8"/>
       <c r="G26" s="47"/>
       <c r="H26" s="44"/>
@@ -8793,7 +8790,7 @@
       <c r="JY26" s="6"/>
       <c r="JZ26" s="6"/>
     </row>
-    <row r="27" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:286">
       <c r="B27" s="8"/>
       <c r="G27" s="47"/>
       <c r="H27" s="44"/>
@@ -9076,7 +9073,7 @@
       <c r="JY27" s="6"/>
       <c r="JZ27" s="6"/>
     </row>
-    <row r="28" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:286">
       <c r="B28" s="8"/>
       <c r="G28" s="47"/>
       <c r="H28" s="44"/>
@@ -9359,7 +9356,7 @@
       <c r="JY28" s="6"/>
       <c r="JZ28" s="6"/>
     </row>
-    <row r="29" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:286">
       <c r="B29" s="8"/>
       <c r="G29" s="47"/>
       <c r="H29" s="44"/>
@@ -9642,7 +9639,7 @@
       <c r="JY29" s="6"/>
       <c r="JZ29" s="6"/>
     </row>
-    <row r="30" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:286">
       <c r="B30" s="8"/>
       <c r="G30" s="47"/>
       <c r="H30" s="44"/>
@@ -9925,7 +9922,7 @@
       <c r="JY30" s="6"/>
       <c r="JZ30" s="6"/>
     </row>
-    <row r="31" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:286">
       <c r="B31" s="8"/>
       <c r="G31" s="47"/>
       <c r="H31" s="44"/>
@@ -10208,7 +10205,7 @@
       <c r="JY31" s="6"/>
       <c r="JZ31" s="6"/>
     </row>
-    <row r="32" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:286">
       <c r="B32" s="8"/>
       <c r="G32" s="47"/>
       <c r="H32" s="44"/>
@@ -10491,7 +10488,7 @@
       <c r="JY32" s="6"/>
       <c r="JZ32" s="6"/>
     </row>
-    <row r="33" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:286">
       <c r="B33" s="8"/>
       <c r="G33" s="47"/>
       <c r="H33" s="44"/>
@@ -10774,7 +10771,7 @@
       <c r="JY33" s="6"/>
       <c r="JZ33" s="6"/>
     </row>
-    <row r="34" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:286">
       <c r="B34" s="8"/>
       <c r="G34" s="47"/>
       <c r="H34" s="44"/>
@@ -11057,7 +11054,7 @@
       <c r="JY34" s="6"/>
       <c r="JZ34" s="6"/>
     </row>
-    <row r="35" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:286">
       <c r="B35" s="8"/>
       <c r="G35" s="47"/>
       <c r="H35" s="44"/>
@@ -11340,7 +11337,7 @@
       <c r="JY35" s="6"/>
       <c r="JZ35" s="6"/>
     </row>
-    <row r="36" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:286">
       <c r="B36" s="8"/>
       <c r="G36" s="47"/>
       <c r="H36" s="44"/>
@@ -11623,7 +11620,7 @@
       <c r="JY36" s="6"/>
       <c r="JZ36" s="6"/>
     </row>
-    <row r="37" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:286">
       <c r="B37" s="8"/>
       <c r="G37" s="47"/>
       <c r="H37" s="44"/>
@@ -11906,7 +11903,7 @@
       <c r="JY37" s="6"/>
       <c r="JZ37" s="6"/>
     </row>
-    <row r="38" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:286">
       <c r="B38" s="8"/>
       <c r="G38" s="47"/>
       <c r="H38" s="44"/>
@@ -12189,7 +12186,7 @@
       <c r="JY38" s="6"/>
       <c r="JZ38" s="6"/>
     </row>
-    <row r="39" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:286">
       <c r="B39" s="8"/>
       <c r="G39" s="47"/>
       <c r="H39" s="44"/>
@@ -12472,7 +12469,7 @@
       <c r="JY39" s="6"/>
       <c r="JZ39" s="6"/>
     </row>
-    <row r="40" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:286">
       <c r="B40" s="8"/>
       <c r="G40" s="47"/>
       <c r="H40" s="44"/>
@@ -12755,7 +12752,7 @@
       <c r="JY40" s="6"/>
       <c r="JZ40" s="6"/>
     </row>
-    <row r="41" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:286">
       <c r="B41" s="8"/>
       <c r="G41" s="47"/>
       <c r="H41" s="44"/>
@@ -13038,7 +13035,7 @@
       <c r="JY41" s="6"/>
       <c r="JZ41" s="6"/>
     </row>
-    <row r="42" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:286">
       <c r="B42" s="8"/>
       <c r="G42" s="47"/>
       <c r="H42" s="44"/>
@@ -13321,7 +13318,7 @@
       <c r="JY42" s="6"/>
       <c r="JZ42" s="6"/>
     </row>
-    <row r="43" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:286">
       <c r="B43" s="8"/>
       <c r="G43" s="47"/>
       <c r="H43" s="44"/>
@@ -13604,7 +13601,7 @@
       <c r="JY43" s="6"/>
       <c r="JZ43" s="6"/>
     </row>
-    <row r="44" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:286">
       <c r="B44" s="8"/>
       <c r="G44" s="47"/>
       <c r="H44" s="44"/>
@@ -13887,7 +13884,7 @@
       <c r="JY44" s="6"/>
       <c r="JZ44" s="6"/>
     </row>
-    <row r="45" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:286">
       <c r="B45" s="8"/>
       <c r="G45" s="47"/>
       <c r="H45" s="44"/>
@@ -14170,7 +14167,7 @@
       <c r="JY45" s="6"/>
       <c r="JZ45" s="6"/>
     </row>
-    <row r="46" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:286">
       <c r="B46" s="8"/>
       <c r="G46" s="47"/>
       <c r="H46" s="44"/>
@@ -14453,7 +14450,7 @@
       <c r="JY46" s="6"/>
       <c r="JZ46" s="6"/>
     </row>
-    <row r="47" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:286">
       <c r="B47" s="8"/>
       <c r="G47" s="47"/>
       <c r="H47" s="44"/>
@@ -14736,7 +14733,7 @@
       <c r="JY47" s="6"/>
       <c r="JZ47" s="6"/>
     </row>
-    <row r="48" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:286">
       <c r="B48" s="8"/>
       <c r="G48" s="47"/>
       <c r="H48" s="44"/>
@@ -15019,7 +15016,7 @@
       <c r="JY48" s="6"/>
       <c r="JZ48" s="6"/>
     </row>
-    <row r="49" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:286">
       <c r="B49" s="8"/>
       <c r="G49" s="47"/>
       <c r="H49" s="44"/>
@@ -15302,7 +15299,7 @@
       <c r="JY49" s="6"/>
       <c r="JZ49" s="6"/>
     </row>
-    <row r="50" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:286">
       <c r="B50" s="8"/>
       <c r="G50" s="47"/>
       <c r="H50" s="44"/>
@@ -15585,7 +15582,7 @@
       <c r="JY50" s="6"/>
       <c r="JZ50" s="6"/>
     </row>
-    <row r="51" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:286">
       <c r="B51" s="8"/>
       <c r="G51" s="47"/>
       <c r="H51" s="44"/>
@@ -15868,7 +15865,7 @@
       <c r="JY51" s="6"/>
       <c r="JZ51" s="6"/>
     </row>
-    <row r="52" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:286">
       <c r="B52" s="8"/>
       <c r="G52" s="47"/>
       <c r="H52" s="44"/>
@@ -16151,7 +16148,7 @@
       <c r="JY52" s="6"/>
       <c r="JZ52" s="6"/>
     </row>
-    <row r="53" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:286">
       <c r="B53" s="8"/>
       <c r="G53" s="47"/>
       <c r="H53" s="44"/>
@@ -16434,7 +16431,7 @@
       <c r="JY53" s="6"/>
       <c r="JZ53" s="6"/>
     </row>
-    <row r="54" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:286">
       <c r="B54" s="8"/>
       <c r="G54" s="47"/>
       <c r="H54" s="44"/>
@@ -16717,7 +16714,7 @@
       <c r="JY54" s="6"/>
       <c r="JZ54" s="6"/>
     </row>
-    <row r="55" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:286">
       <c r="B55" s="8"/>
       <c r="G55" s="47"/>
       <c r="H55" s="44"/>
@@ -17000,7 +16997,7 @@
       <c r="JY55" s="6"/>
       <c r="JZ55" s="6"/>
     </row>
-    <row r="56" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:286">
       <c r="B56" s="8"/>
       <c r="G56" s="47"/>
       <c r="H56" s="44"/>
@@ -17283,7 +17280,7 @@
       <c r="JY56" s="6"/>
       <c r="JZ56" s="6"/>
     </row>
-    <row r="57" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:286">
       <c r="B57" s="8"/>
       <c r="G57" s="47"/>
       <c r="H57" s="44"/>
@@ -17566,7 +17563,7 @@
       <c r="JY57" s="6"/>
       <c r="JZ57" s="6"/>
     </row>
-    <row r="58" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:286">
       <c r="B58" s="8"/>
       <c r="G58" s="47"/>
       <c r="H58" s="44"/>
@@ -17849,7 +17846,7 @@
       <c r="JY58" s="6"/>
       <c r="JZ58" s="6"/>
     </row>
-    <row r="59" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:286">
       <c r="B59" s="8"/>
       <c r="G59" s="47"/>
       <c r="H59" s="44"/>
@@ -18132,7 +18129,7 @@
       <c r="JY59" s="6"/>
       <c r="JZ59" s="6"/>
     </row>
-    <row r="60" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:286">
       <c r="B60" s="8"/>
       <c r="G60" s="47"/>
       <c r="H60" s="44"/>
@@ -18415,7 +18412,7 @@
       <c r="JY60" s="6"/>
       <c r="JZ60" s="6"/>
     </row>
-    <row r="61" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:286">
       <c r="B61" s="8"/>
       <c r="G61" s="47"/>
       <c r="H61" s="44"/>
@@ -18698,7 +18695,7 @@
       <c r="JY61" s="6"/>
       <c r="JZ61" s="6"/>
     </row>
-    <row r="62" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:286">
       <c r="B62" s="8"/>
       <c r="G62" s="47"/>
       <c r="H62" s="44"/>
@@ -18981,7 +18978,7 @@
       <c r="JY62" s="6"/>
       <c r="JZ62" s="6"/>
     </row>
-    <row r="63" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:286">
       <c r="B63" s="8"/>
       <c r="G63" s="47"/>
       <c r="H63" s="44"/>
@@ -19264,7 +19261,7 @@
       <c r="JY63" s="6"/>
       <c r="JZ63" s="6"/>
     </row>
-    <row r="64" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:286">
       <c r="B64" s="8"/>
       <c r="G64" s="47"/>
       <c r="H64" s="44"/>
@@ -19547,7 +19544,7 @@
       <c r="JY64" s="6"/>
       <c r="JZ64" s="6"/>
     </row>
-    <row r="65" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:286">
       <c r="B65" s="8"/>
       <c r="G65" s="47"/>
       <c r="H65" s="44"/>
@@ -19830,7 +19827,7 @@
       <c r="JY65" s="6"/>
       <c r="JZ65" s="6"/>
     </row>
-    <row r="66" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:286">
       <c r="B66" s="8"/>
       <c r="G66" s="47"/>
       <c r="H66" s="44"/>
@@ -20113,7 +20110,7 @@
       <c r="JY66" s="6"/>
       <c r="JZ66" s="6"/>
     </row>
-    <row r="67" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:286">
       <c r="B67" s="8"/>
       <c r="G67" s="47"/>
       <c r="H67" s="44"/>
@@ -20396,7 +20393,7 @@
       <c r="JY67" s="6"/>
       <c r="JZ67" s="6"/>
     </row>
-    <row r="68" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:286">
       <c r="B68" s="8"/>
       <c r="G68" s="47"/>
       <c r="H68" s="44"/>
@@ -20679,7 +20676,7 @@
       <c r="JY68" s="6"/>
       <c r="JZ68" s="6"/>
     </row>
-    <row r="69" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:286">
       <c r="B69" s="8"/>
       <c r="G69" s="47"/>
       <c r="H69" s="44"/>
@@ -20962,7 +20959,7 @@
       <c r="JY69" s="6"/>
       <c r="JZ69" s="6"/>
     </row>
-    <row r="70" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:286">
       <c r="B70" s="8"/>
       <c r="G70" s="47"/>
       <c r="H70" s="44"/>
@@ -21245,7 +21242,7 @@
       <c r="JY70" s="6"/>
       <c r="JZ70" s="6"/>
     </row>
-    <row r="71" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:286">
       <c r="B71" s="11"/>
       <c r="G71" s="47"/>
       <c r="H71" s="44"/>
@@ -21528,7 +21525,7 @@
       <c r="JY71" s="6"/>
       <c r="JZ71" s="6"/>
     </row>
-    <row r="72" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:286">
       <c r="B72" s="11"/>
       <c r="G72" s="47"/>
       <c r="H72" s="44"/>
@@ -21811,7 +21808,7 @@
       <c r="JY72" s="6"/>
       <c r="JZ72" s="6"/>
     </row>
-    <row r="73" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:286">
       <c r="B73" s="11"/>
       <c r="G73" s="47"/>
       <c r="H73" s="44"/>
@@ -22094,7 +22091,7 @@
       <c r="JY73" s="6"/>
       <c r="JZ73" s="6"/>
     </row>
-    <row r="74" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:286">
       <c r="B74" s="11"/>
       <c r="G74" s="47"/>
       <c r="H74" s="44"/>
@@ -22377,7 +22374,7 @@
       <c r="JY74" s="6"/>
       <c r="JZ74" s="6"/>
     </row>
-    <row r="75" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:286">
       <c r="B75" s="11"/>
       <c r="G75" s="47"/>
       <c r="H75" s="44"/>
@@ -22660,7 +22657,7 @@
       <c r="JY75" s="6"/>
       <c r="JZ75" s="6"/>
     </row>
-    <row r="76" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:286">
       <c r="B76" s="11"/>
       <c r="G76" s="47"/>
       <c r="H76" s="44"/>
@@ -22943,7 +22940,7 @@
       <c r="JY76" s="6"/>
       <c r="JZ76" s="6"/>
     </row>
-    <row r="77" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:286">
       <c r="B77" s="11"/>
       <c r="G77" s="47"/>
       <c r="H77" s="44"/>
@@ -23226,7 +23223,7 @@
       <c r="JY77" s="6"/>
       <c r="JZ77" s="6"/>
     </row>
-    <row r="78" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:286">
       <c r="B78" s="11"/>
       <c r="G78" s="47"/>
       <c r="H78" s="44"/>
@@ -23509,7 +23506,7 @@
       <c r="JY78" s="6"/>
       <c r="JZ78" s="6"/>
     </row>
-    <row r="79" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:286">
       <c r="B79" s="11"/>
       <c r="G79" s="47"/>
       <c r="H79" s="44"/>
@@ -23792,7 +23789,7 @@
       <c r="JY79" s="6"/>
       <c r="JZ79" s="6"/>
     </row>
-    <row r="80" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:286">
       <c r="B80" s="11"/>
       <c r="G80" s="47"/>
       <c r="H80" s="44"/>
@@ -24075,7 +24072,7 @@
       <c r="JY80" s="6"/>
       <c r="JZ80" s="6"/>
     </row>
-    <row r="81" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:286">
       <c r="B81" s="11"/>
       <c r="G81" s="47"/>
       <c r="H81" s="44"/>
@@ -24358,7 +24355,7 @@
       <c r="JY81" s="6"/>
       <c r="JZ81" s="6"/>
     </row>
-    <row r="82" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:286">
       <c r="B82" s="11"/>
       <c r="G82" s="47"/>
       <c r="H82" s="44"/>
@@ -24641,7 +24638,7 @@
       <c r="JY82" s="6"/>
       <c r="JZ82" s="6"/>
     </row>
-    <row r="83" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:286">
       <c r="B83" s="11"/>
       <c r="G83" s="47"/>
       <c r="H83" s="44"/>
@@ -24924,7 +24921,7 @@
       <c r="JY83" s="6"/>
       <c r="JZ83" s="6"/>
     </row>
-    <row r="84" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:286">
       <c r="B84" s="11"/>
       <c r="G84" s="47"/>
       <c r="H84" s="44"/>
@@ -25207,7 +25204,7 @@
       <c r="JY84" s="6"/>
       <c r="JZ84" s="6"/>
     </row>
-    <row r="85" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:286">
       <c r="B85" s="11"/>
       <c r="G85" s="47"/>
       <c r="H85" s="44"/>
@@ -25490,7 +25487,7 @@
       <c r="JY85" s="6"/>
       <c r="JZ85" s="6"/>
     </row>
-    <row r="86" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:286">
       <c r="B86" s="11"/>
       <c r="G86" s="47"/>
       <c r="H86" s="44"/>
@@ -25773,7 +25770,7 @@
       <c r="JY86" s="6"/>
       <c r="JZ86" s="6"/>
     </row>
-    <row r="87" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:286">
       <c r="B87" s="11"/>
       <c r="G87" s="47"/>
       <c r="H87" s="44"/>
@@ -26056,7 +26053,7 @@
       <c r="JY87" s="6"/>
       <c r="JZ87" s="6"/>
     </row>
-    <row r="88" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:286">
       <c r="B88" s="11"/>
       <c r="G88" s="47"/>
       <c r="H88" s="44"/>
@@ -26339,7 +26336,7 @@
       <c r="JY88" s="6"/>
       <c r="JZ88" s="6"/>
     </row>
-    <row r="89" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:286">
       <c r="B89" s="11"/>
       <c r="G89" s="47"/>
       <c r="H89" s="44"/>
@@ -26622,7 +26619,7 @@
       <c r="JY89" s="6"/>
       <c r="JZ89" s="6"/>
     </row>
-    <row r="90" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:286">
       <c r="B90" s="11"/>
       <c r="G90" s="47"/>
       <c r="H90" s="44"/>
@@ -26905,7 +26902,7 @@
       <c r="JY90" s="6"/>
       <c r="JZ90" s="6"/>
     </row>
-    <row r="91" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:286">
       <c r="B91" s="11"/>
       <c r="G91" s="47"/>
       <c r="H91" s="44"/>
@@ -27188,7 +27185,7 @@
       <c r="JY91" s="6"/>
       <c r="JZ91" s="6"/>
     </row>
-    <row r="92" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:286">
       <c r="B92" s="11"/>
       <c r="G92" s="47"/>
       <c r="H92" s="44"/>
@@ -27471,7 +27468,7 @@
       <c r="JY92" s="6"/>
       <c r="JZ92" s="6"/>
     </row>
-    <row r="93" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:286">
       <c r="B93" s="11"/>
       <c r="G93" s="47"/>
       <c r="H93" s="44"/>
@@ -27754,7 +27751,7 @@
       <c r="JY93" s="6"/>
       <c r="JZ93" s="6"/>
     </row>
-    <row r="94" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:286">
       <c r="B94" s="11"/>
       <c r="G94" s="47"/>
       <c r="H94" s="44"/>
@@ -28037,7 +28034,7 @@
       <c r="JY94" s="6"/>
       <c r="JZ94" s="6"/>
     </row>
-    <row r="95" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:286">
       <c r="B95" s="11"/>
       <c r="G95" s="47"/>
       <c r="H95" s="44"/>
@@ -28320,7 +28317,7 @@
       <c r="JY95" s="6"/>
       <c r="JZ95" s="6"/>
     </row>
-    <row r="96" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:286">
       <c r="B96" s="11"/>
       <c r="G96" s="47"/>
       <c r="H96" s="44"/>
@@ -28603,7 +28600,7 @@
       <c r="JY96" s="6"/>
       <c r="JZ96" s="6"/>
     </row>
-    <row r="97" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:286">
       <c r="B97" s="11"/>
       <c r="G97" s="47"/>
       <c r="H97" s="44"/>
@@ -28886,7 +28883,7 @@
       <c r="JY97" s="6"/>
       <c r="JZ97" s="6"/>
     </row>
-    <row r="98" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:286">
       <c r="B98" s="11"/>
       <c r="G98" s="47"/>
       <c r="H98" s="44"/>
@@ -29169,7 +29166,7 @@
       <c r="JY98" s="6"/>
       <c r="JZ98" s="6"/>
     </row>
-    <row r="99" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:286">
       <c r="B99" s="11"/>
       <c r="G99" s="47"/>
       <c r="H99" s="44"/>
@@ -29452,7 +29449,7 @@
       <c r="JY99" s="6"/>
       <c r="JZ99" s="6"/>
     </row>
-    <row r="100" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:286">
       <c r="B100" s="11"/>
       <c r="G100" s="47"/>
       <c r="H100" s="44"/>
@@ -29735,7 +29732,7 @@
       <c r="JY100" s="6"/>
       <c r="JZ100" s="6"/>
     </row>
-    <row r="101" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:286">
       <c r="B101" s="11"/>
       <c r="G101" s="47"/>
       <c r="H101" s="44"/>
@@ -30018,7 +30015,7 @@
       <c r="JY101" s="6"/>
       <c r="JZ101" s="6"/>
     </row>
-    <row r="102" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:286">
       <c r="B102" s="11"/>
       <c r="G102" s="47"/>
       <c r="H102" s="44"/>
@@ -30301,7 +30298,7 @@
       <c r="JY102" s="6"/>
       <c r="JZ102" s="6"/>
     </row>
-    <row r="103" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:286">
       <c r="B103" s="11"/>
       <c r="G103" s="47"/>
       <c r="H103" s="44"/>
@@ -30584,7 +30581,7 @@
       <c r="JY103" s="6"/>
       <c r="JZ103" s="6"/>
     </row>
-    <row r="104" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:286">
       <c r="B104" s="11"/>
       <c r="G104" s="47"/>
       <c r="H104" s="44"/>
@@ -30867,7 +30864,7 @@
       <c r="JY104" s="6"/>
       <c r="JZ104" s="6"/>
     </row>
-    <row r="105" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:286">
       <c r="B105" s="11"/>
       <c r="G105" s="47"/>
       <c r="H105" s="44"/>
@@ -31150,7 +31147,7 @@
       <c r="JY105" s="6"/>
       <c r="JZ105" s="6"/>
     </row>
-    <row r="106" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:286">
       <c r="B106" s="11"/>
       <c r="G106" s="47"/>
       <c r="H106" s="44"/>
@@ -31433,7 +31430,7 @@
       <c r="JY106" s="6"/>
       <c r="JZ106" s="6"/>
     </row>
-    <row r="107" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:286">
       <c r="B107" s="11"/>
       <c r="G107" s="47"/>
       <c r="H107" s="44"/>
@@ -31716,7 +31713,7 @@
       <c r="JY107" s="6"/>
       <c r="JZ107" s="6"/>
     </row>
-    <row r="108" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:286">
       <c r="B108" s="11"/>
       <c r="G108" s="47"/>
       <c r="H108" s="44"/>
@@ -31999,7 +31996,7 @@
       <c r="JY108" s="6"/>
       <c r="JZ108" s="6"/>
     </row>
-    <row r="109" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:286">
       <c r="B109" s="11"/>
       <c r="G109" s="47"/>
       <c r="H109" s="44"/>
@@ -32282,7 +32279,7 @@
       <c r="JY109" s="6"/>
       <c r="JZ109" s="6"/>
     </row>
-    <row r="110" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:286">
       <c r="B110" s="11"/>
       <c r="G110" s="47"/>
       <c r="H110" s="44"/>
@@ -32565,7 +32562,7 @@
       <c r="JY110" s="6"/>
       <c r="JZ110" s="6"/>
     </row>
-    <row r="111" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:286">
       <c r="B111" s="11"/>
       <c r="G111" s="47"/>
       <c r="H111" s="44"/>
@@ -32848,7 +32845,7 @@
       <c r="JY111" s="6"/>
       <c r="JZ111" s="6"/>
     </row>
-    <row r="112" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:286">
       <c r="B112" s="11"/>
       <c r="G112" s="47"/>
       <c r="H112" s="44"/>
@@ -33131,7 +33128,7 @@
       <c r="JY112" s="6"/>
       <c r="JZ112" s="6"/>
     </row>
-    <row r="113" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:286">
       <c r="B113" s="11"/>
       <c r="G113" s="47"/>
       <c r="H113" s="44"/>
@@ -33414,7 +33411,7 @@
       <c r="JY113" s="6"/>
       <c r="JZ113" s="6"/>
     </row>
-    <row r="114" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:286">
       <c r="B114" s="11"/>
       <c r="G114" s="47"/>
       <c r="H114" s="44"/>
@@ -33697,7 +33694,7 @@
       <c r="JY114" s="6"/>
       <c r="JZ114" s="6"/>
     </row>
-    <row r="115" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:286">
       <c r="B115" s="11"/>
       <c r="G115" s="47"/>
       <c r="H115" s="44"/>
@@ -33980,7 +33977,7 @@
       <c r="JY115" s="6"/>
       <c r="JZ115" s="6"/>
     </row>
-    <row r="116" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:286">
       <c r="B116" s="11"/>
       <c r="G116" s="47"/>
       <c r="H116" s="44"/>
@@ -34263,7 +34260,7 @@
       <c r="JY116" s="6"/>
       <c r="JZ116" s="6"/>
     </row>
-    <row r="117" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:286">
       <c r="B117" s="11"/>
       <c r="G117" s="47"/>
       <c r="H117" s="44"/>
@@ -34546,7 +34543,7 @@
       <c r="JY117" s="6"/>
       <c r="JZ117" s="6"/>
     </row>
-    <row r="118" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:286">
       <c r="B118" s="11"/>
       <c r="G118" s="47"/>
       <c r="H118" s="44"/>
@@ -34829,7 +34826,7 @@
       <c r="JY118" s="6"/>
       <c r="JZ118" s="6"/>
     </row>
-    <row r="119" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:286">
       <c r="B119" s="11"/>
       <c r="G119" s="47"/>
       <c r="H119" s="44"/>
@@ -35112,7 +35109,7 @@
       <c r="JY119" s="6"/>
       <c r="JZ119" s="6"/>
     </row>
-    <row r="120" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:286">
       <c r="B120" s="11"/>
       <c r="G120" s="47"/>
       <c r="H120" s="44"/>
@@ -35395,7 +35392,7 @@
       <c r="JY120" s="6"/>
       <c r="JZ120" s="6"/>
     </row>
-    <row r="121" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:286">
       <c r="B121" s="11"/>
       <c r="G121" s="47"/>
       <c r="H121" s="44"/>
@@ -35678,7 +35675,7 @@
       <c r="JY121" s="6"/>
       <c r="JZ121" s="6"/>
     </row>
-    <row r="122" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:286">
       <c r="B122" s="11"/>
       <c r="G122" s="47"/>
       <c r="H122" s="44"/>
@@ -35961,7 +35958,7 @@
       <c r="JY122" s="6"/>
       <c r="JZ122" s="6"/>
     </row>
-    <row r="123" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:286">
       <c r="B123" s="11"/>
       <c r="G123" s="47"/>
       <c r="H123" s="44"/>
@@ -36244,7 +36241,7 @@
       <c r="JY123" s="6"/>
       <c r="JZ123" s="6"/>
     </row>
-    <row r="124" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:286">
       <c r="B124" s="11"/>
       <c r="G124" s="47"/>
       <c r="H124" s="44"/>
@@ -36527,7 +36524,7 @@
       <c r="JY124" s="6"/>
       <c r="JZ124" s="6"/>
     </row>
-    <row r="125" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:286">
       <c r="B125" s="11"/>
       <c r="G125" s="47"/>
       <c r="H125" s="44"/>
@@ -36810,7 +36807,7 @@
       <c r="JY125" s="6"/>
       <c r="JZ125" s="6"/>
     </row>
-    <row r="126" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:286">
       <c r="B126" s="11"/>
       <c r="G126" s="47"/>
       <c r="H126" s="44"/>
@@ -37093,7 +37090,7 @@
       <c r="JY126" s="6"/>
       <c r="JZ126" s="6"/>
     </row>
-    <row r="127" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:286">
       <c r="B127" s="11"/>
       <c r="G127" s="47"/>
       <c r="H127" s="44"/>
@@ -37376,7 +37373,7 @@
       <c r="JY127" s="6"/>
       <c r="JZ127" s="6"/>
     </row>
-    <row r="128" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:286">
       <c r="B128" s="11"/>
       <c r="G128" s="47"/>
       <c r="H128" s="44"/>
@@ -37659,7 +37656,7 @@
       <c r="JY128" s="6"/>
       <c r="JZ128" s="6"/>
     </row>
-    <row r="129" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:286">
       <c r="B129" s="11"/>
       <c r="G129" s="47"/>
       <c r="H129" s="44"/>
@@ -37942,7 +37939,7 @@
       <c r="JY129" s="6"/>
       <c r="JZ129" s="6"/>
     </row>
-    <row r="130" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:286">
       <c r="B130" s="11"/>
       <c r="G130" s="47"/>
       <c r="H130" s="44"/>
@@ -38225,7 +38222,7 @@
       <c r="JY130" s="6"/>
       <c r="JZ130" s="6"/>
     </row>
-    <row r="131" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:286">
       <c r="B131" s="11"/>
       <c r="G131" s="47"/>
       <c r="H131" s="44"/>
@@ -38508,7 +38505,7 @@
       <c r="JY131" s="6"/>
       <c r="JZ131" s="6"/>
     </row>
-    <row r="132" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:286">
       <c r="B132" s="11"/>
       <c r="G132" s="47"/>
       <c r="H132" s="44"/>
@@ -38791,7 +38788,7 @@
       <c r="JY132" s="6"/>
       <c r="JZ132" s="6"/>
     </row>
-    <row r="133" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:286">
       <c r="B133" s="11"/>
       <c r="G133" s="47"/>
       <c r="H133" s="44"/>
@@ -39074,7 +39071,7 @@
       <c r="JY133" s="6"/>
       <c r="JZ133" s="6"/>
     </row>
-    <row r="134" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:286">
       <c r="B134" s="11"/>
       <c r="G134" s="47"/>
       <c r="H134" s="44"/>
@@ -39357,7 +39354,7 @@
       <c r="JY134" s="6"/>
       <c r="JZ134" s="6"/>
     </row>
-    <row r="135" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:286">
       <c r="B135" s="11"/>
       <c r="G135" s="47"/>
       <c r="H135" s="44"/>
@@ -39640,7 +39637,7 @@
       <c r="JY135" s="6"/>
       <c r="JZ135" s="6"/>
     </row>
-    <row r="136" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:286">
       <c r="B136" s="11"/>
       <c r="G136" s="47"/>
       <c r="H136" s="44"/>
@@ -39923,7 +39920,7 @@
       <c r="JY136" s="6"/>
       <c r="JZ136" s="6"/>
     </row>
-    <row r="137" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:286">
       <c r="B137" s="11"/>
       <c r="G137" s="47"/>
       <c r="H137" s="44"/>
@@ -40206,7 +40203,7 @@
       <c r="JY137" s="6"/>
       <c r="JZ137" s="6"/>
     </row>
-    <row r="138" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:286">
       <c r="B138" s="11"/>
       <c r="G138" s="47"/>
       <c r="H138" s="44"/>
@@ -40489,7 +40486,7 @@
       <c r="JY138" s="6"/>
       <c r="JZ138" s="6"/>
     </row>
-    <row r="139" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:286">
       <c r="B139" s="11"/>
       <c r="G139" s="47"/>
       <c r="H139" s="44"/>
@@ -40772,7 +40769,7 @@
       <c r="JY139" s="6"/>
       <c r="JZ139" s="6"/>
     </row>
-    <row r="140" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:286">
       <c r="B140" s="11"/>
       <c r="G140" s="47"/>
       <c r="H140" s="44"/>
@@ -41055,7 +41052,7 @@
       <c r="JY140" s="6"/>
       <c r="JZ140" s="6"/>
     </row>
-    <row r="141" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:286">
       <c r="B141" s="11"/>
       <c r="G141" s="47"/>
       <c r="H141" s="44"/>
@@ -41338,7 +41335,7 @@
       <c r="JY141" s="6"/>
       <c r="JZ141" s="6"/>
     </row>
-    <row r="142" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:286">
       <c r="B142" s="11"/>
       <c r="G142" s="47"/>
       <c r="H142" s="44"/>
@@ -41621,7 +41618,7 @@
       <c r="JY142" s="6"/>
       <c r="JZ142" s="6"/>
     </row>
-    <row r="143" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:286">
       <c r="B143" s="11"/>
       <c r="G143" s="47"/>
       <c r="H143" s="44"/>
@@ -41904,7 +41901,7 @@
       <c r="JY143" s="6"/>
       <c r="JZ143" s="6"/>
     </row>
-    <row r="144" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:286">
       <c r="B144" s="11"/>
       <c r="G144" s="47"/>
       <c r="H144" s="44"/>
@@ -42187,7 +42184,7 @@
       <c r="JY144" s="6"/>
       <c r="JZ144" s="6"/>
     </row>
-    <row r="145" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:286">
       <c r="B145" s="11"/>
       <c r="G145" s="47"/>
       <c r="H145" s="44"/>
@@ -42470,7 +42467,7 @@
       <c r="JY145" s="6"/>
       <c r="JZ145" s="6"/>
     </row>
-    <row r="146" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:286">
       <c r="B146" s="11"/>
       <c r="G146" s="47"/>
       <c r="H146" s="44"/>
@@ -42753,7 +42750,7 @@
       <c r="JY146" s="6"/>
       <c r="JZ146" s="6"/>
     </row>
-    <row r="147" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:286">
       <c r="B147" s="11"/>
       <c r="G147" s="47"/>
       <c r="H147" s="44"/>
@@ -43036,7 +43033,7 @@
       <c r="JY147" s="6"/>
       <c r="JZ147" s="6"/>
     </row>
-    <row r="148" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:286">
       <c r="B148" s="11"/>
       <c r="G148" s="47"/>
       <c r="H148" s="44"/>
@@ -43319,7 +43316,7 @@
       <c r="JY148" s="6"/>
       <c r="JZ148" s="6"/>
     </row>
-    <row r="149" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:286">
       <c r="B149" s="11"/>
       <c r="G149" s="47"/>
       <c r="H149" s="44"/>
@@ -43602,7 +43599,7 @@
       <c r="JY149" s="6"/>
       <c r="JZ149" s="6"/>
     </row>
-    <row r="150" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:286">
       <c r="B150" s="11"/>
       <c r="G150" s="47"/>
       <c r="H150" s="44"/>
@@ -43885,7 +43882,7 @@
       <c r="JY150" s="6"/>
       <c r="JZ150" s="6"/>
     </row>
-    <row r="151" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:286">
       <c r="B151" s="11"/>
       <c r="G151" s="47"/>
       <c r="H151" s="44"/>
@@ -44168,7 +44165,7 @@
       <c r="JY151" s="6"/>
       <c r="JZ151" s="6"/>
     </row>
-    <row r="152" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:286">
       <c r="B152" s="11"/>
       <c r="G152" s="47"/>
       <c r="H152" s="44"/>
@@ -44451,7 +44448,7 @@
       <c r="JY152" s="6"/>
       <c r="JZ152" s="6"/>
     </row>
-    <row r="153" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:286">
       <c r="B153" s="11"/>
       <c r="G153" s="47"/>
       <c r="H153" s="44"/>
@@ -44734,7 +44731,7 @@
       <c r="JY153" s="6"/>
       <c r="JZ153" s="6"/>
     </row>
-    <row r="154" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:286">
       <c r="B154" s="11"/>
       <c r="G154" s="47"/>
       <c r="H154" s="44"/>
@@ -45017,7 +45014,7 @@
       <c r="JY154" s="6"/>
       <c r="JZ154" s="6"/>
     </row>
-    <row r="155" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:286">
       <c r="B155" s="11"/>
       <c r="G155" s="47"/>
       <c r="H155" s="44"/>
@@ -45300,7 +45297,7 @@
       <c r="JY155" s="6"/>
       <c r="JZ155" s="6"/>
     </row>
-    <row r="156" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:286">
       <c r="B156" s="11"/>
       <c r="G156" s="47"/>
       <c r="H156" s="44"/>
@@ -45583,7 +45580,7 @@
       <c r="JY156" s="6"/>
       <c r="JZ156" s="6"/>
     </row>
-    <row r="157" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:286">
       <c r="B157" s="11"/>
       <c r="G157" s="47"/>
       <c r="H157" s="44"/>
@@ -45866,7 +45863,7 @@
       <c r="JY157" s="6"/>
       <c r="JZ157" s="6"/>
     </row>
-    <row r="158" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:286">
       <c r="B158" s="11"/>
       <c r="G158" s="47"/>
       <c r="H158" s="44"/>
@@ -46149,7 +46146,7 @@
       <c r="JY158" s="6"/>
       <c r="JZ158" s="6"/>
     </row>
-    <row r="159" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:286">
       <c r="B159" s="11"/>
       <c r="G159" s="47"/>
       <c r="H159" s="44"/>
@@ -46432,7 +46429,7 @@
       <c r="JY159" s="6"/>
       <c r="JZ159" s="6"/>
     </row>
-    <row r="160" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:286">
       <c r="B160" s="11"/>
       <c r="G160" s="47"/>
       <c r="H160" s="44"/>
@@ -46715,7 +46712,7 @@
       <c r="JY160" s="6"/>
       <c r="JZ160" s="6"/>
     </row>
-    <row r="161" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:286">
       <c r="B161" s="11"/>
       <c r="G161" s="47"/>
       <c r="H161" s="44"/>
@@ -46998,7 +46995,7 @@
       <c r="JY161" s="6"/>
       <c r="JZ161" s="6"/>
     </row>
-    <row r="162" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:286">
       <c r="B162" s="11"/>
       <c r="G162" s="47"/>
       <c r="H162" s="44"/>
@@ -47281,7 +47278,7 @@
       <c r="JY162" s="6"/>
       <c r="JZ162" s="6"/>
     </row>
-    <row r="163" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:286">
       <c r="B163" s="11"/>
       <c r="G163" s="47"/>
       <c r="H163" s="44"/>
@@ -47564,7 +47561,7 @@
       <c r="JY163" s="6"/>
       <c r="JZ163" s="6"/>
     </row>
-    <row r="164" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:286">
       <c r="B164" s="11"/>
       <c r="G164" s="47"/>
       <c r="H164" s="44"/>
@@ -47847,7 +47844,7 @@
       <c r="JY164" s="6"/>
       <c r="JZ164" s="6"/>
     </row>
-    <row r="165" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:286">
       <c r="B165" s="11"/>
       <c r="G165" s="47"/>
       <c r="H165" s="44"/>
@@ -48130,7 +48127,7 @@
       <c r="JY165" s="6"/>
       <c r="JZ165" s="6"/>
     </row>
-    <row r="166" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:286">
       <c r="B166" s="11"/>
       <c r="G166" s="47"/>
       <c r="H166" s="44"/>
@@ -48413,7 +48410,7 @@
       <c r="JY166" s="6"/>
       <c r="JZ166" s="6"/>
     </row>
-    <row r="167" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:286">
       <c r="B167" s="11"/>
       <c r="G167" s="47"/>
       <c r="H167" s="44"/>
@@ -48696,7 +48693,7 @@
       <c r="JY167" s="6"/>
       <c r="JZ167" s="6"/>
     </row>
-    <row r="168" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:286">
       <c r="B168" s="11"/>
       <c r="G168" s="47"/>
       <c r="H168" s="44"/>
@@ -48979,7 +48976,7 @@
       <c r="JY168" s="6"/>
       <c r="JZ168" s="6"/>
     </row>
-    <row r="169" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:286">
       <c r="B169" s="11"/>
       <c r="G169" s="47"/>
       <c r="H169" s="44"/>
@@ -49262,7 +49259,7 @@
       <c r="JY169" s="6"/>
       <c r="JZ169" s="6"/>
     </row>
-    <row r="170" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:286">
       <c r="B170" s="11"/>
       <c r="G170" s="47"/>
       <c r="H170" s="44"/>
@@ -49545,7 +49542,7 @@
       <c r="JY170" s="6"/>
       <c r="JZ170" s="6"/>
     </row>
-    <row r="171" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:286">
       <c r="B171" s="11"/>
       <c r="G171" s="47"/>
       <c r="H171" s="44"/>
@@ -49828,7 +49825,7 @@
       <c r="JY171" s="6"/>
       <c r="JZ171" s="6"/>
     </row>
-    <row r="172" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:286">
       <c r="B172" s="11"/>
       <c r="G172" s="47"/>
       <c r="H172" s="44"/>
@@ -50111,7 +50108,7 @@
       <c r="JY172" s="6"/>
       <c r="JZ172" s="6"/>
     </row>
-    <row r="173" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:286">
       <c r="B173" s="11"/>
       <c r="G173" s="47"/>
       <c r="H173" s="44"/>
@@ -50394,7 +50391,7 @@
       <c r="JY173" s="6"/>
       <c r="JZ173" s="6"/>
     </row>
-    <row r="174" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:286">
       <c r="B174" s="11"/>
       <c r="G174" s="47"/>
       <c r="H174" s="44"/>
@@ -50677,7 +50674,7 @@
       <c r="JY174" s="6"/>
       <c r="JZ174" s="6"/>
     </row>
-    <row r="175" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:286">
       <c r="B175" s="11"/>
       <c r="G175" s="47"/>
       <c r="H175" s="44"/>
@@ -50960,7 +50957,7 @@
       <c r="JY175" s="6"/>
       <c r="JZ175" s="6"/>
     </row>
-    <row r="176" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:286">
       <c r="B176" s="11"/>
       <c r="G176" s="47"/>
       <c r="H176" s="44"/>
@@ -51243,7 +51240,7 @@
       <c r="JY176" s="6"/>
       <c r="JZ176" s="6"/>
     </row>
-    <row r="177" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:286">
       <c r="B177" s="11"/>
       <c r="G177" s="47"/>
       <c r="H177" s="44"/>
@@ -51526,7 +51523,7 @@
       <c r="JY177" s="6"/>
       <c r="JZ177" s="6"/>
     </row>
-    <row r="178" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:286">
       <c r="B178" s="11"/>
       <c r="G178" s="47"/>
       <c r="H178" s="44"/>
@@ -51809,7 +51806,7 @@
       <c r="JY178" s="6"/>
       <c r="JZ178" s="6"/>
     </row>
-    <row r="179" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:286">
       <c r="B179" s="11"/>
       <c r="G179" s="47"/>
       <c r="H179" s="44"/>
@@ -52092,7 +52089,7 @@
       <c r="JY179" s="6"/>
       <c r="JZ179" s="6"/>
     </row>
-    <row r="180" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:286">
       <c r="B180" s="11"/>
       <c r="G180" s="47"/>
       <c r="H180" s="44"/>
@@ -52375,7 +52372,7 @@
       <c r="JY180" s="6"/>
       <c r="JZ180" s="6"/>
     </row>
-    <row r="181" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:286">
       <c r="B181" s="11"/>
       <c r="G181" s="47"/>
       <c r="H181" s="44"/>
@@ -52658,7 +52655,7 @@
       <c r="JY181" s="6"/>
       <c r="JZ181" s="6"/>
     </row>
-    <row r="182" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:286">
       <c r="B182" s="11"/>
       <c r="G182" s="47"/>
       <c r="H182" s="44"/>
@@ -52941,7 +52938,7 @@
       <c r="JY182" s="6"/>
       <c r="JZ182" s="6"/>
     </row>
-    <row r="183" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:286">
       <c r="B183" s="11"/>
       <c r="G183" s="47"/>
       <c r="H183" s="44"/>
@@ -53224,7 +53221,7 @@
       <c r="JY183" s="6"/>
       <c r="JZ183" s="6"/>
     </row>
-    <row r="184" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:286">
       <c r="B184" s="11"/>
       <c r="G184" s="47"/>
       <c r="H184" s="44"/>
@@ -53507,7 +53504,7 @@
       <c r="JY184" s="6"/>
       <c r="JZ184" s="6"/>
     </row>
-    <row r="185" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:286">
       <c r="B185" s="11"/>
       <c r="G185" s="47"/>
       <c r="H185" s="44"/>
@@ -53790,7 +53787,7 @@
       <c r="JY185" s="6"/>
       <c r="JZ185" s="6"/>
     </row>
-    <row r="186" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:286">
       <c r="B186" s="11"/>
       <c r="G186" s="47"/>
       <c r="H186" s="44"/>
@@ -54073,7 +54070,7 @@
       <c r="JY186" s="6"/>
       <c r="JZ186" s="6"/>
     </row>
-    <row r="187" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:286">
       <c r="B187" s="11"/>
       <c r="G187" s="47"/>
       <c r="H187" s="44"/>
@@ -54356,7 +54353,7 @@
       <c r="JY187" s="6"/>
       <c r="JZ187" s="6"/>
     </row>
-    <row r="188" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:286">
       <c r="B188" s="11"/>
       <c r="G188" s="47"/>
       <c r="H188" s="44"/>
@@ -54639,7 +54636,7 @@
       <c r="JY188" s="6"/>
       <c r="JZ188" s="6"/>
     </row>
-    <row r="189" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:286">
       <c r="B189" s="11"/>
       <c r="G189" s="47"/>
       <c r="H189" s="44"/>
@@ -54922,7 +54919,7 @@
       <c r="JY189" s="6"/>
       <c r="JZ189" s="6"/>
     </row>
-    <row r="190" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:286">
       <c r="B190" s="11"/>
       <c r="G190" s="47"/>
       <c r="H190" s="44"/>
@@ -55205,7 +55202,7 @@
       <c r="JY190" s="6"/>
       <c r="JZ190" s="6"/>
     </row>
-    <row r="191" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:286">
       <c r="B191" s="11"/>
       <c r="G191" s="47"/>
       <c r="H191" s="44"/>
@@ -55488,7 +55485,7 @@
       <c r="JY191" s="6"/>
       <c r="JZ191" s="6"/>
     </row>
-    <row r="192" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:286">
       <c r="B192" s="11"/>
       <c r="G192" s="47"/>
       <c r="H192" s="44"/>
@@ -55771,7 +55768,7 @@
       <c r="JY192" s="6"/>
       <c r="JZ192" s="6"/>
     </row>
-    <row r="193" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:286">
       <c r="B193" s="11"/>
       <c r="G193" s="47"/>
       <c r="H193" s="44"/>
@@ -56054,7 +56051,7 @@
       <c r="JY193" s="6"/>
       <c r="JZ193" s="6"/>
     </row>
-    <row r="194" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:286">
       <c r="B194" s="11"/>
       <c r="G194" s="47"/>
       <c r="H194" s="44"/>
@@ -56337,7 +56334,7 @@
       <c r="JY194" s="6"/>
       <c r="JZ194" s="6"/>
     </row>
-    <row r="195" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:286">
       <c r="B195" s="11"/>
       <c r="G195" s="47"/>
       <c r="H195" s="44"/>
@@ -56620,7 +56617,7 @@
       <c r="JY195" s="6"/>
       <c r="JZ195" s="6"/>
     </row>
-    <row r="196" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:286">
       <c r="B196" s="11"/>
       <c r="G196" s="47"/>
       <c r="H196" s="44"/>
@@ -56903,7 +56900,7 @@
       <c r="JY196" s="6"/>
       <c r="JZ196" s="6"/>
     </row>
-    <row r="197" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:286">
       <c r="B197" s="11"/>
       <c r="G197" s="47"/>
       <c r="H197" s="44"/>
@@ -57186,7 +57183,7 @@
       <c r="JY197" s="6"/>
       <c r="JZ197" s="6"/>
     </row>
-    <row r="198" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:286">
       <c r="B198" s="11"/>
       <c r="G198" s="47"/>
       <c r="H198" s="44"/>
@@ -57469,7 +57466,7 @@
       <c r="JY198" s="6"/>
       <c r="JZ198" s="6"/>
     </row>
-    <row r="199" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:286">
       <c r="B199" s="11"/>
       <c r="G199" s="47"/>
       <c r="H199" s="44"/>
@@ -57752,7 +57749,7 @@
       <c r="JY199" s="6"/>
       <c r="JZ199" s="6"/>
     </row>
-    <row r="200" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:286">
       <c r="B200" s="11"/>
       <c r="G200" s="47"/>
       <c r="H200" s="44"/>
@@ -58035,7 +58032,7 @@
       <c r="JY200" s="6"/>
       <c r="JZ200" s="6"/>
     </row>
-    <row r="201" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:286">
       <c r="B201" s="11"/>
       <c r="G201" s="47"/>
       <c r="H201" s="44"/>
@@ -58318,7 +58315,7 @@
       <c r="JY201" s="6"/>
       <c r="JZ201" s="6"/>
     </row>
-    <row r="202" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:286">
       <c r="B202" s="11"/>
       <c r="G202" s="47"/>
       <c r="H202" s="44"/>
@@ -58601,7 +58598,7 @@
       <c r="JY202" s="6"/>
       <c r="JZ202" s="6"/>
     </row>
-    <row r="203" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:286">
       <c r="B203" s="11"/>
       <c r="G203" s="47"/>
       <c r="H203" s="44"/>
@@ -58884,7 +58881,7 @@
       <c r="JY203" s="6"/>
       <c r="JZ203" s="6"/>
     </row>
-    <row r="204" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:286">
       <c r="B204" s="11"/>
       <c r="G204" s="47"/>
       <c r="H204" s="44"/>
@@ -59167,7 +59164,7 @@
       <c r="JY204" s="6"/>
       <c r="JZ204" s="6"/>
     </row>
-    <row r="205" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:286">
       <c r="B205" s="11"/>
       <c r="G205" s="47"/>
       <c r="H205" s="44"/>
@@ -59450,7 +59447,7 @@
       <c r="JY205" s="6"/>
       <c r="JZ205" s="6"/>
     </row>
-    <row r="206" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:286">
       <c r="B206" s="11"/>
       <c r="G206" s="47"/>
       <c r="H206" s="44"/>
@@ -59733,7 +59730,7 @@
       <c r="JY206" s="6"/>
       <c r="JZ206" s="6"/>
     </row>
-    <row r="207" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:286">
       <c r="B207" s="11"/>
       <c r="G207" s="47"/>
       <c r="H207" s="44"/>
@@ -60016,7 +60013,7 @@
       <c r="JY207" s="6"/>
       <c r="JZ207" s="6"/>
     </row>
-    <row r="208" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:286">
       <c r="B208" s="11"/>
       <c r="G208" s="47"/>
       <c r="H208" s="44"/>
@@ -60299,7 +60296,7 @@
       <c r="JY208" s="6"/>
       <c r="JZ208" s="6"/>
     </row>
-    <row r="209" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:286">
       <c r="B209" s="11"/>
       <c r="G209" s="47"/>
       <c r="H209" s="44"/>
@@ -60582,7 +60579,7 @@
       <c r="JY209" s="6"/>
       <c r="JZ209" s="6"/>
     </row>
-    <row r="210" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:286">
       <c r="B210" s="11"/>
       <c r="G210" s="47"/>
       <c r="H210" s="44"/>
@@ -60865,7 +60862,7 @@
       <c r="JY210" s="6"/>
       <c r="JZ210" s="6"/>
     </row>
-    <row r="211" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:286">
       <c r="B211" s="11"/>
       <c r="G211" s="47"/>
       <c r="H211" s="44"/>
@@ -61148,7 +61145,7 @@
       <c r="JY211" s="6"/>
       <c r="JZ211" s="6"/>
     </row>
-    <row r="212" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:286">
       <c r="B212" s="11"/>
       <c r="G212" s="47"/>
       <c r="H212" s="44"/>
@@ -61431,7 +61428,7 @@
       <c r="JY212" s="6"/>
       <c r="JZ212" s="6"/>
     </row>
-    <row r="213" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:286">
       <c r="B213" s="11"/>
       <c r="G213" s="47"/>
       <c r="H213" s="44"/>
@@ -61714,7 +61711,7 @@
       <c r="JY213" s="6"/>
       <c r="JZ213" s="6"/>
     </row>
-    <row r="214" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:286">
       <c r="B214" s="11"/>
       <c r="G214" s="47"/>
       <c r="H214" s="44"/>
@@ -61997,7 +61994,7 @@
       <c r="JY214" s="6"/>
       <c r="JZ214" s="6"/>
     </row>
-    <row r="215" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:286">
       <c r="B215" s="11"/>
       <c r="G215" s="47"/>
       <c r="H215" s="44"/>
@@ -62280,7 +62277,7 @@
       <c r="JY215" s="6"/>
       <c r="JZ215" s="6"/>
     </row>
-    <row r="216" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:286">
       <c r="B216" s="11"/>
       <c r="G216" s="47"/>
       <c r="H216" s="44"/>
@@ -62563,7 +62560,7 @@
       <c r="JY216" s="6"/>
       <c r="JZ216" s="6"/>
     </row>
-    <row r="217" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:286">
       <c r="B217" s="11"/>
       <c r="G217" s="47"/>
       <c r="H217" s="44"/>
@@ -62846,7 +62843,7 @@
       <c r="JY217" s="6"/>
       <c r="JZ217" s="6"/>
     </row>
-    <row r="218" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:286">
       <c r="B218" s="11"/>
       <c r="G218" s="47"/>
       <c r="H218" s="44"/>
@@ -63129,7 +63126,7 @@
       <c r="JY218" s="6"/>
       <c r="JZ218" s="6"/>
     </row>
-    <row r="219" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:286">
       <c r="B219" s="11"/>
       <c r="G219" s="47"/>
       <c r="H219" s="44"/>
@@ -63412,7 +63409,7 @@
       <c r="JY219" s="6"/>
       <c r="JZ219" s="6"/>
     </row>
-    <row r="220" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:286">
       <c r="B220" s="11"/>
       <c r="G220" s="47"/>
       <c r="H220" s="44"/>
@@ -63695,7 +63692,7 @@
       <c r="JY220" s="6"/>
       <c r="JZ220" s="6"/>
     </row>
-    <row r="221" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:286">
       <c r="B221" s="11"/>
       <c r="G221" s="47"/>
       <c r="H221" s="44"/>
@@ -63978,157 +63975,157 @@
       <c r="JY221" s="6"/>
       <c r="JZ221" s="6"/>
     </row>
-    <row r="222" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:286">
       <c r="B222" s="4"/>
       <c r="G222"/>
     </row>
-    <row r="223" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:286">
       <c r="B223" s="4"/>
       <c r="G223"/>
     </row>
-    <row r="224" spans="2:286" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:286">
       <c r="B224" s="4"/>
       <c r="G224"/>
     </row>
-    <row r="225" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:7">
       <c r="B225" s="4"/>
       <c r="G225"/>
     </row>
-    <row r="226" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:7">
       <c r="B226" s="4"/>
       <c r="G226"/>
     </row>
-    <row r="227" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:7">
       <c r="B227" s="4"/>
       <c r="G227"/>
     </row>
-    <row r="228" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:7">
       <c r="B228" s="4"/>
       <c r="G228"/>
     </row>
-    <row r="229" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:7">
       <c r="B229" s="4"/>
       <c r="G229"/>
     </row>
-    <row r="230" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:7">
       <c r="B230" s="4"/>
       <c r="G230"/>
     </row>
-    <row r="231" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:7">
       <c r="B231" s="4"/>
       <c r="G231"/>
     </row>
-    <row r="232" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:7">
       <c r="B232" s="4"/>
       <c r="G232"/>
     </row>
-    <row r="233" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:7">
       <c r="B233" s="4"/>
       <c r="G233"/>
     </row>
-    <row r="234" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:7">
       <c r="B234" s="4"/>
       <c r="G234"/>
     </row>
-    <row r="235" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:7">
       <c r="B235" s="4"/>
       <c r="G235"/>
     </row>
-    <row r="236" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:7">
       <c r="B236" s="4"/>
       <c r="G236"/>
     </row>
-    <row r="237" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:7">
       <c r="B237" s="4"/>
       <c r="G237"/>
     </row>
-    <row r="238" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="238" spans="2:7">
       <c r="B238" s="4"/>
       <c r="G238"/>
     </row>
-    <row r="239" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="239" spans="2:7">
       <c r="B239" s="4"/>
       <c r="G239"/>
     </row>
-    <row r="240" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="240" spans="2:7">
       <c r="B240" s="4"/>
       <c r="G240"/>
     </row>
-    <row r="241" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="241" spans="2:7">
       <c r="B241" s="4"/>
       <c r="G241"/>
     </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="242" spans="2:7">
       <c r="B242" s="4"/>
       <c r="G242"/>
     </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:7">
       <c r="B243" s="4"/>
       <c r="G243"/>
     </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:7">
       <c r="B244" s="4"/>
       <c r="G244"/>
     </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:7">
       <c r="B245" s="4"/>
       <c r="G245"/>
     </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:7">
       <c r="B246" s="4"/>
     </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:7">
       <c r="B247" s="4"/>
     </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="248" spans="2:7">
       <c r="B248" s="4"/>
     </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:7">
       <c r="B249" s="4"/>
     </row>
-    <row r="250" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:7">
       <c r="B250" s="4"/>
     </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:7">
       <c r="B251" s="4"/>
     </row>
-    <row r="252" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:7">
       <c r="B252" s="4"/>
     </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:7">
       <c r="B253" s="4"/>
     </row>
-    <row r="254" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:7">
       <c r="B254" s="4"/>
     </row>
-    <row r="255" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:7">
       <c r="B255" s="4"/>
     </row>
-    <row r="256" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:7">
       <c r="B256" s="4"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="2:2">
       <c r="B257" s="4"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:2">
       <c r="B258" s="4"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="2:2">
       <c r="B259" s="4"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="2:2">
       <c r="B260" s="4"/>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="2:2">
       <c r="B261" s="4"/>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="2:2">
       <c r="B262" s="4"/>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="2:2">
       <c r="B263" s="4"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="2:2">
       <c r="B264" s="4"/>
     </row>
   </sheetData>
@@ -64164,6 +64161,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008E38A6EF0D87AA46993DD52020FE3E27" ma:contentTypeVersion="4" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="dfe1cc72eea7af3507f75b45ca8c569c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a042ee54-f02a-415e-9595-341646dc5167" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ecb1440112991bebd2e886ca4acac8bd" ns2:_="">
     <xsd:import namespace="a042ee54-f02a-415e-9595-341646dc5167"/>
@@ -64307,15 +64313,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -64323,6 +64320,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7222CD-4E52-4DCB-A6D9-A689C06F8147}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD64B337-4DCE-4E01-973F-6CCC399E27D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -64336,14 +64341,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7222CD-4E52-4DCB-A6D9-A689C06F8147}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Plot changes to fit all covid legends, and creation of acmap_HA_H6N2 with H6N2 and removal of H6N2 from original dataset.
</commit_message>
<xml_diff>
--- a/data/_raw/acmap_NA.xlsx
+++ b/data/_raw/acmap_NA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hilarius\OneDrive - Danmarks Tekniske Universitet\Dokumenter\Antigenic-Mapping-of-NA\data\_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2FCB27-CED5-431A-9410-F7EECD974B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36AC6A7-A6CC-44B3-8D0B-DAA1CA62097B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>Made by;                                                                OLSE &amp; MAOJ, 2024</t>
   </si>
@@ -180,9 +180,6 @@
     <t>H6N1 A/CA/04/2009/N1 (H1N1)</t>
   </si>
   <si>
-    <t>H6N2 A/Texas/50/2012(4) (H3N2)</t>
-  </si>
-  <si>
     <t>Richard Webby's lab</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
   </si>
   <si>
     <t>H6N1</t>
-  </si>
-  <si>
-    <t>H6N2</t>
   </si>
   <si>
     <t>Serum vaccine homolog:</t>
@@ -241,9 +235,6 @@
   </si>
   <si>
     <t>Challenge wt H1N1</t>
-  </si>
-  <si>
-    <t>Unrelated rec H6N2</t>
   </si>
 </sst>
 </file>
@@ -602,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -724,9 +715,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1079,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:HW264"/>
+  <dimension ref="A1:HW263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1102,23 +1090,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:231" s="5" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
     </row>
     <row r="2" spans="1:231" s="4" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:231" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1131,13 +1119,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1603,13 +1591,13 @@
         <v>5</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -2325,76 +2313,76 @@
         <v>9</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="U9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="W9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="X9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Y9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Z9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AA9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AB9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AC9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AD9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AE9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AF9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:231" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -2405,79 +2393,79 @@
       <c r="F10" s="4"/>
       <c r="G10" s="36"/>
       <c r="H10" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="Z10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="AA10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="AB10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="AC10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="AD10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="AE10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="AF10" s="35" t="s">
         <v>59</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y10" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z10" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA10" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB10" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC10" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD10" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE10" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF10" s="35" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:231" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2776,7 +2764,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H12" s="40" t="s">
         <v>15</v>
@@ -3007,20 +2995,20 @@
     <row r="13" spans="1:231" x14ac:dyDescent="0.35">
       <c r="B13" s="8"/>
       <c r="C13" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I13" s="13">
         <v>648.4</v>
@@ -3303,13 +3291,13 @@
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I14" s="13">
         <v>487.4</v>
@@ -3585,18 +3573,18 @@
     <row r="15" spans="1:231" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="8"/>
       <c r="C15" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I15" s="13">
         <v>198.6</v>
@@ -3872,88 +3860,90 @@
     <row r="16" spans="1:231" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
-      <c r="G16" s="45"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="41" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I16" s="13">
-        <v>45.3</v>
+        <v>499.9</v>
       </c>
       <c r="J16" s="13">
-        <v>23.8</v>
+        <v>194.7</v>
       </c>
       <c r="K16" s="13">
-        <v>46.6</v>
+        <v>149.30000000000001</v>
       </c>
       <c r="L16" s="13">
-        <v>44.6</v>
+        <v>100.9</v>
       </c>
       <c r="M16" s="13">
-        <v>43.1</v>
+        <v>108.8</v>
       </c>
       <c r="N16" s="13">
-        <v>45.5</v>
+        <v>316.5</v>
       </c>
       <c r="O16" s="13">
-        <v>45.5</v>
+        <v>319.10000000000002</v>
       </c>
       <c r="P16" s="13">
-        <v>48</v>
+        <v>283</v>
       </c>
       <c r="Q16" s="13">
-        <v>23.4</v>
+        <v>593.70000000000005</v>
       </c>
       <c r="R16" s="13">
-        <v>46</v>
+        <v>306.8</v>
       </c>
       <c r="S16" s="13">
-        <v>26.3</v>
+        <v>459</v>
       </c>
       <c r="T16" s="13">
-        <v>24.6</v>
+        <v>225.1</v>
       </c>
       <c r="U16" s="13">
-        <v>24.1</v>
+        <v>193.5</v>
       </c>
       <c r="V16" s="13">
-        <v>23.4</v>
+        <v>171.2</v>
       </c>
       <c r="W16" s="13">
-        <v>23.9</v>
+        <v>344.6</v>
       </c>
       <c r="X16" s="13">
-        <v>12.9</v>
+        <v>459.9</v>
       </c>
       <c r="Y16" s="13">
-        <v>15.1</v>
+        <v>1390.2</v>
       </c>
-      <c r="Z16" s="47"/>
+      <c r="Z16" s="13">
+        <v>2913.8</v>
+      </c>
       <c r="AA16" s="13">
-        <v>15.1</v>
+        <v>1785.8</v>
       </c>
       <c r="AB16" s="13">
-        <v>15.1</v>
+        <v>1476.4</v>
       </c>
       <c r="AC16" s="13">
-        <v>25.2</v>
+        <v>2126.6</v>
       </c>
       <c r="AD16" s="13">
-        <v>22</v>
+        <v>3343</v>
       </c>
       <c r="AE16" s="13">
-        <v>26</v>
+        <v>5696.4</v>
       </c>
       <c r="AF16" s="13">
-        <v>29.4</v>
+        <v>6454.6</v>
       </c>
       <c r="AG16" s="13"/>
       <c r="AH16" s="13"/>
@@ -4154,103 +4144,47 @@
       <c r="HU16" s="6"/>
       <c r="HV16" s="6"/>
     </row>
-    <row r="17" spans="2:230" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:230" x14ac:dyDescent="0.35">
       <c r="B17" s="8"/>
-      <c r="C17" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="13">
-        <v>499.9</v>
-      </c>
-      <c r="J17" s="13">
-        <v>194.7</v>
-      </c>
-      <c r="K17" s="13">
-        <v>149.30000000000001</v>
-      </c>
-      <c r="L17" s="13">
-        <v>100.9</v>
-      </c>
-      <c r="M17" s="13">
-        <v>108.8</v>
-      </c>
-      <c r="N17" s="13">
-        <v>316.5</v>
-      </c>
-      <c r="O17" s="13">
-        <v>319.10000000000002</v>
-      </c>
-      <c r="P17" s="13">
-        <v>283</v>
-      </c>
-      <c r="Q17" s="13">
-        <v>593.70000000000005</v>
-      </c>
-      <c r="R17" s="13">
-        <v>306.8</v>
-      </c>
-      <c r="S17" s="13">
-        <v>459</v>
-      </c>
-      <c r="T17" s="13">
-        <v>225.1</v>
-      </c>
-      <c r="U17" s="13">
-        <v>193.5</v>
-      </c>
-      <c r="V17" s="13">
-        <v>171.2</v>
-      </c>
-      <c r="W17" s="13">
-        <v>344.6</v>
-      </c>
-      <c r="X17" s="13">
-        <v>459.9</v>
-      </c>
-      <c r="Y17" s="13">
-        <v>1390.2</v>
-      </c>
-      <c r="Z17" s="13">
-        <v>2913.8</v>
-      </c>
-      <c r="AA17" s="13">
-        <v>1785.8</v>
-      </c>
-      <c r="AB17" s="13">
-        <v>1476.4</v>
-      </c>
-      <c r="AC17" s="13">
-        <v>2126.6</v>
-      </c>
-      <c r="AD17" s="13">
-        <v>3343</v>
-      </c>
-      <c r="AE17" s="13">
-        <v>5696.4</v>
-      </c>
-      <c r="AF17" s="13">
-        <v>6454.6</v>
-      </c>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="13"/>
-      <c r="AJ17" s="13"/>
-      <c r="AK17" s="13"/>
-      <c r="AL17" s="13"/>
-      <c r="AM17" s="13"/>
-      <c r="AN17" s="13"/>
-      <c r="AO17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="6"/>
+      <c r="AL17" s="6"/>
+      <c r="AM17" s="6"/>
+      <c r="AN17" s="6"/>
+      <c r="AO17" s="6"/>
       <c r="AP17" s="6"/>
       <c r="AQ17" s="6"/>
       <c r="AR17" s="6"/>
@@ -5139,7 +5073,7 @@
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="45"/>
       <c r="H21" s="41"/>
       <c r="I21" s="6"/>
@@ -5367,12 +5301,8 @@
     </row>
     <row r="22" spans="2:230" x14ac:dyDescent="0.35">
       <c r="B22" s="8"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="31"/>
       <c r="G22" s="45"/>
-      <c r="H22" s="41"/>
+      <c r="H22" s="42"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -16266,7 +16196,7 @@
       <c r="HV69" s="6"/>
     </row>
     <row r="70" spans="2:230" x14ac:dyDescent="0.35">
-      <c r="B70" s="8"/>
+      <c r="B70" s="11"/>
       <c r="G70" s="45"/>
       <c r="H70" s="42"/>
       <c r="I70" s="6"/>
@@ -50543,231 +50473,8 @@
       <c r="HV220" s="6"/>
     </row>
     <row r="221" spans="2:230" x14ac:dyDescent="0.35">
-      <c r="B221" s="11"/>
-      <c r="G221" s="45"/>
-      <c r="H221" s="42"/>
-      <c r="I221" s="6"/>
-      <c r="J221" s="6"/>
-      <c r="K221" s="6"/>
-      <c r="L221" s="6"/>
-      <c r="M221" s="6"/>
-      <c r="N221" s="6"/>
-      <c r="O221" s="6"/>
-      <c r="P221" s="6"/>
-      <c r="Q221" s="6"/>
-      <c r="R221" s="6"/>
-      <c r="S221" s="6"/>
-      <c r="T221" s="6"/>
-      <c r="U221" s="6"/>
-      <c r="V221" s="6"/>
-      <c r="W221" s="6"/>
-      <c r="X221" s="6"/>
-      <c r="Y221" s="6"/>
-      <c r="Z221" s="6"/>
-      <c r="AA221" s="6"/>
-      <c r="AB221" s="6"/>
-      <c r="AC221" s="6"/>
-      <c r="AD221" s="6"/>
-      <c r="AE221" s="6"/>
-      <c r="AF221" s="6"/>
-      <c r="AG221" s="6"/>
-      <c r="AH221" s="6"/>
-      <c r="AI221" s="6"/>
-      <c r="AJ221" s="6"/>
-      <c r="AK221" s="6"/>
-      <c r="AL221" s="6"/>
-      <c r="AM221" s="6"/>
-      <c r="AN221" s="6"/>
-      <c r="AO221" s="6"/>
-      <c r="AP221" s="6"/>
-      <c r="AQ221" s="6"/>
-      <c r="AR221" s="6"/>
-      <c r="AS221" s="6"/>
-      <c r="AT221" s="6"/>
-      <c r="AU221" s="6"/>
-      <c r="AV221" s="6"/>
-      <c r="AW221" s="6"/>
-      <c r="AX221" s="6"/>
-      <c r="AY221" s="6"/>
-      <c r="AZ221" s="6"/>
-      <c r="BA221" s="6"/>
-      <c r="BB221" s="6"/>
-      <c r="BC221" s="6"/>
-      <c r="BD221" s="6"/>
-      <c r="BE221" s="6"/>
-      <c r="BF221" s="6"/>
-      <c r="BG221" s="6"/>
-      <c r="BH221" s="6"/>
-      <c r="BI221" s="6"/>
-      <c r="BJ221" s="6"/>
-      <c r="BK221" s="6"/>
-      <c r="BL221" s="6"/>
-      <c r="BM221" s="6"/>
-      <c r="BN221" s="6"/>
-      <c r="BO221" s="6"/>
-      <c r="BP221" s="6"/>
-      <c r="BQ221" s="6"/>
-      <c r="BR221" s="6"/>
-      <c r="BS221" s="6"/>
-      <c r="BT221" s="6"/>
-      <c r="BU221" s="6"/>
-      <c r="BV221" s="6"/>
-      <c r="BW221" s="6"/>
-      <c r="BX221" s="6"/>
-      <c r="BY221" s="6"/>
-      <c r="BZ221" s="6"/>
-      <c r="CA221" s="6"/>
-      <c r="CB221" s="6"/>
-      <c r="CC221" s="6"/>
-      <c r="CD221" s="6"/>
-      <c r="CE221" s="6"/>
-      <c r="CF221" s="6"/>
-      <c r="CG221" s="6"/>
-      <c r="CH221" s="6"/>
-      <c r="CI221" s="6"/>
-      <c r="CJ221" s="6"/>
-      <c r="CK221" s="6"/>
-      <c r="CL221" s="6"/>
-      <c r="CM221" s="6"/>
-      <c r="CN221" s="6"/>
-      <c r="CO221" s="6"/>
-      <c r="CP221" s="6"/>
-      <c r="CQ221" s="6"/>
-      <c r="CR221" s="6"/>
-      <c r="CS221" s="6"/>
-      <c r="CT221" s="6"/>
-      <c r="CU221" s="6"/>
-      <c r="CV221" s="6"/>
-      <c r="CW221" s="6"/>
-      <c r="CX221" s="6"/>
-      <c r="CY221" s="6"/>
-      <c r="CZ221" s="6"/>
-      <c r="DA221" s="6"/>
-      <c r="DB221" s="6"/>
-      <c r="DC221" s="6"/>
-      <c r="DD221" s="6"/>
-      <c r="DE221" s="6"/>
-      <c r="DF221" s="6"/>
-      <c r="DG221" s="6"/>
-      <c r="DH221" s="6"/>
-      <c r="DI221" s="6"/>
-      <c r="DJ221" s="6"/>
-      <c r="DK221" s="6"/>
-      <c r="DL221" s="6"/>
-      <c r="DM221" s="6"/>
-      <c r="DN221" s="6"/>
-      <c r="DO221" s="6"/>
-      <c r="DP221" s="6"/>
-      <c r="DQ221" s="6"/>
-      <c r="DR221" s="6"/>
-      <c r="DS221" s="6"/>
-      <c r="DT221" s="6"/>
-      <c r="DU221" s="6"/>
-      <c r="DV221" s="6"/>
-      <c r="DW221" s="6"/>
-      <c r="DX221" s="6"/>
-      <c r="DY221" s="6"/>
-      <c r="DZ221" s="6"/>
-      <c r="EA221" s="6"/>
-      <c r="EB221" s="6"/>
-      <c r="EC221" s="6"/>
-      <c r="ED221" s="6"/>
-      <c r="EE221" s="6"/>
-      <c r="EF221" s="6"/>
-      <c r="EG221" s="6"/>
-      <c r="EH221" s="6"/>
-      <c r="EI221" s="6"/>
-      <c r="EJ221" s="6"/>
-      <c r="EK221" s="6"/>
-      <c r="EL221" s="6"/>
-      <c r="EM221" s="6"/>
-      <c r="EN221" s="6"/>
-      <c r="EO221" s="6"/>
-      <c r="EP221" s="6"/>
-      <c r="EQ221" s="6"/>
-      <c r="ER221" s="6"/>
-      <c r="ES221" s="6"/>
-      <c r="ET221" s="6"/>
-      <c r="EU221" s="6"/>
-      <c r="EV221" s="6"/>
-      <c r="EW221" s="6"/>
-      <c r="EX221" s="6"/>
-      <c r="EY221" s="6"/>
-      <c r="EZ221" s="6"/>
-      <c r="FA221" s="6"/>
-      <c r="FB221" s="6"/>
-      <c r="FC221" s="6"/>
-      <c r="FD221" s="6"/>
-      <c r="FE221" s="6"/>
-      <c r="FF221" s="6"/>
-      <c r="FG221" s="6"/>
-      <c r="FH221" s="6"/>
-      <c r="FI221" s="6"/>
-      <c r="FJ221" s="6"/>
-      <c r="FK221" s="6"/>
-      <c r="FL221" s="6"/>
-      <c r="FM221" s="6"/>
-      <c r="FN221" s="6"/>
-      <c r="FO221" s="6"/>
-      <c r="FP221" s="6"/>
-      <c r="FQ221" s="6"/>
-      <c r="FR221" s="6"/>
-      <c r="FS221" s="6"/>
-      <c r="FT221" s="6"/>
-      <c r="FU221" s="6"/>
-      <c r="FV221" s="6"/>
-      <c r="FW221" s="6"/>
-      <c r="FX221" s="6"/>
-      <c r="FY221" s="6"/>
-      <c r="FZ221" s="6"/>
-      <c r="GA221" s="6"/>
-      <c r="GB221" s="6"/>
-      <c r="GC221" s="6"/>
-      <c r="GD221" s="6"/>
-      <c r="GE221" s="6"/>
-      <c r="GF221" s="6"/>
-      <c r="GG221" s="6"/>
-      <c r="GH221" s="6"/>
-      <c r="GI221" s="6"/>
-      <c r="GJ221" s="6"/>
-      <c r="GK221" s="6"/>
-      <c r="GL221" s="6"/>
-      <c r="GM221" s="6"/>
-      <c r="GN221" s="6"/>
-      <c r="GO221" s="6"/>
-      <c r="GP221" s="6"/>
-      <c r="GQ221" s="6"/>
-      <c r="GR221" s="6"/>
-      <c r="GS221" s="6"/>
-      <c r="GT221" s="6"/>
-      <c r="GU221" s="6"/>
-      <c r="GV221" s="6"/>
-      <c r="GW221" s="6"/>
-      <c r="GX221" s="6"/>
-      <c r="GY221" s="6"/>
-      <c r="GZ221" s="6"/>
-      <c r="HA221" s="6"/>
-      <c r="HB221" s="6"/>
-      <c r="HC221" s="6"/>
-      <c r="HD221" s="6"/>
-      <c r="HE221" s="6"/>
-      <c r="HF221" s="6"/>
-      <c r="HG221" s="6"/>
-      <c r="HH221" s="6"/>
-      <c r="HI221" s="6"/>
-      <c r="HJ221" s="6"/>
-      <c r="HK221" s="6"/>
-      <c r="HL221" s="6"/>
-      <c r="HM221" s="6"/>
-      <c r="HN221" s="6"/>
-      <c r="HO221" s="6"/>
-      <c r="HP221" s="6"/>
-      <c r="HQ221" s="6"/>
-      <c r="HR221" s="6"/>
-      <c r="HS221" s="6"/>
-      <c r="HT221" s="6"/>
-      <c r="HU221" s="6"/>
-      <c r="HV221" s="6"/>
+      <c r="B221" s="4"/>
+      <c r="G221"/>
     </row>
     <row r="222" spans="2:230" x14ac:dyDescent="0.35">
       <c r="B222" s="4"/>
@@ -50863,7 +50570,6 @@
     </row>
     <row r="245" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B245" s="4"/>
-      <c r="G245"/>
     </row>
     <row r="246" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B246" s="4"/>
@@ -50919,9 +50625,6 @@
     <row r="263" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B263" s="4"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B264" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
@@ -50934,19 +50637,19 @@
       <formula1>45363</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert file path here" prompt="Copy file path from &quot;File Explorer&quot; and paste it here. This is where the plots, report and Racmacs interface. " sqref="C7" xr:uid="{27B9733A-C5B7-4500-B65E-95C3FA937881}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="(optional) Insert strain origin" prompt="In the format of: _x000a_&lt;virus type and subtype/origin/strain number/year isolated&gt; _x000a_An example could be; &lt;seasonal influenza A(H3N2)/Perth/16/2019&gt;" sqref="D13:D221" xr:uid="{07E23837-5D22-427F-B224-D5B1FA90F7C0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="(optional) Insert SSI name" prompt="Insert the name the antigen is known as within the SSI system. " sqref="E13:E221" xr:uid="{0DA7DC1C-F230-4A91-9D52-E83BB5DE063D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert antigenic group" prompt="IMPORTANT: If an antigen in use corresponds to the antigen in &quot;Serum exposure&quot;, proceed to write it here identically to &quot;Serum exposure:&quot;_x000a_Beyond that, the idea is to write e.g. &quot;Delta&quot; at each instance of Delta variant in a COVID dataset. " sqref="F13:F221" xr:uid="{194C4819-7700-47AB-A9FA-060C5A8AC6F1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert antigens" prompt="Write the names of the antigens, which the serum has been tested against." sqref="H13:H221" xr:uid="{6CF6A8D4-2D02-4415-B8C1-32E3002E3245}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert Serum IDs" prompt="Paste here the ID's of all your serum samples. " sqref="I11:HV11" xr:uid="{401F2837-386A-4170-BBA1-F7E1A77EF1F3}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert protein of interest" prompt="Write here the name of the viral protein (e.g. neuraminidase)._x000a_Can NOT be left empty." sqref="F5" xr:uid="{09BE6BBA-F97F-4B17-A736-EF3536D87F14}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert name of assay" prompt="Insert name (preferably abbreviation) of assay in use (e.g. ELLA)._x000a_Should NOT be left empty." sqref="H3" xr:uid="{9684EE06-8694-4828-9CF5-149254120E51}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert species name" prompt="Put here the species which the serum samples are from (e.g. pig)._x000a_Both latin and english name works. " sqref="H5" xr:uid="{1C14AD12-4143-4DA0-8B36-63A0B46BE1F5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="(optional) Insert antigen comment" prompt="Paste notes for the antigen tested for, or leave it blank. " sqref="C13:C221 E13" xr:uid="{7151EE93-E9FC-4DEF-B1D5-46169D6B6973}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="(optional) Insert antigen comment" prompt="Paste notes for the antigen tested for, or leave it blank. " sqref="E13 C13:C220" xr:uid="{7151EE93-E9FC-4DEF-B1D5-46169D6B6973}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert serum exposure" prompt="Insert the name of the antigen which the serum have been exposed to, and developed antibodies against. _x000a_IMPORTANT: If an antigen in use corresponds to the antigen in &quot;Serum exposure&quot;, proceed to write it here identically to &quot;Antigenic group:&quot; " sqref="I10:HV10" xr:uid="{E5F7D863-CDA1-4F0E-B520-93DCA51039C1}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="(optional) serum notes" prompt="Paste notes for the serum samples. _x000a_Can be left empty " sqref="I8:HV8" xr:uid="{599DFA9D-8F67-4359-8566-78CEFAF888C2}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="(optional) Days Post Inoculation" prompt="Insert here the serum DPI._x000a_Can be left empty. " sqref="I9:HV9" xr:uid="{ABBA3676-7881-4C8A-81E8-F3FEB997EEDC}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Inhibition Titer" prompt="Insert here inhibition titer for the serum samples and the corresponding antigen. _x000a_Can be left EMPTY." sqref="I13:HV221" xr:uid="{BE0D63C4-7B0D-4DBE-BB25-5DFB0542CC50}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="(optional) Insert strain origin" prompt="In the format of: _x000a_&lt;virus type and subtype/origin/strain number/year isolated&gt; _x000a_An example could be; &lt;seasonal influenza A(H3N2)/Perth/16/2019&gt;" sqref="D13:D220" xr:uid="{07E23837-5D22-427F-B224-D5B1FA90F7C0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="(optional) Insert SSI name" prompt="Insert the name the antigen is known as within the SSI system. " sqref="E13:E220" xr:uid="{0DA7DC1C-F230-4A91-9D52-E83BB5DE063D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert antigenic group" prompt="IMPORTANT: If an antigen in use corresponds to the antigen in &quot;Serum exposure&quot;, proceed to write it here identically to &quot;Serum exposure:&quot;_x000a_Beyond that, the idea is to write e.g. &quot;Delta&quot; at each instance of Delta variant in a COVID dataset. " sqref="F13:F220" xr:uid="{194C4819-7700-47AB-A9FA-060C5A8AC6F1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Insert antigens" prompt="Write the names of the antigens, which the serum has been tested against." sqref="H13:H220" xr:uid="{6CF6A8D4-2D02-4415-B8C1-32E3002E3245}"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Inhibition Titer" prompt="Insert here inhibition titer for the serum samples and the corresponding antigen. _x000a_Can be left EMPTY." sqref="I13:HV220" xr:uid="{BE0D63C4-7B0D-4DBE-BB25-5DFB0542CC50}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -50955,6 +50658,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008E38A6EF0D87AA46993DD52020FE3E27" ma:contentTypeVersion="4" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="dfe1cc72eea7af3507f75b45ca8c569c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a042ee54-f02a-415e-9595-341646dc5167" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ecb1440112991bebd2e886ca4acac8bd" ns2:_="">
     <xsd:import namespace="a042ee54-f02a-415e-9595-341646dc5167"/>
@@ -51098,15 +50810,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -51114,6 +50817,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7222CD-4E52-4DCB-A6D9-A689C06F8147}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD64B337-4DCE-4E01-973F-6CCC399E27D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -51127,14 +50838,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7222CD-4E52-4DCB-A6D9-A689C06F8147}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>